<commit_message>
creasion de la prueba 1
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AGUIRRE\Desktop\TAREAS\Mravi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492EDE7F-4F96-4119-B8F6-0754C231868E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,8 +24,19 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Hola muchachos</t>
+  </si>
+  <si>
+    <t>Ronfis</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +347,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
creasion de la prueba 3
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1e6551fc873be8c6/Escritorio/codico uda/Mravi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AGUIRRE\Desktop\TAREAS\Mravi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{492EDE7F-4F96-4119-B8F6-0754C231868E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D542363A-66AA-4780-8B73-C0F65B5CE75D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EADECF-F5A7-4A9A-B2C8-07794E9BA69F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -89,6 +89,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1" descr="Los 25 paisajes más bonitos del mundo: imágenes reales">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E82BD7CF-8320-464B-A9CE-70273D219F10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4267200" y="1280160"/>
+          <a:ext cx="1965960" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,12 +423,12 @@
   <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -370,7 +436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -380,5 +446,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>